<commit_message>
fixed decimal point issue
</commit_message>
<xml_diff>
--- a/coordinates.xlsx
+++ b/coordinates.xlsx
@@ -15,6 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0000000000"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -32,7 +35,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +43,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,59 +366,59 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
+      <c r="A1" s="1">
+        <v>-0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>-0</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
-        <v>-1.976896614795781</v>
-      </c>
-      <c r="B2">
-        <v>0.3031167669545516</v>
+      <c r="A2" s="1">
+        <v>-1.917462659138496</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-0.5686272512019883</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
-        <v>-2.510419294117958</v>
-      </c>
-      <c r="B3">
-        <v>3.420203936420769</v>
+      <c r="A3" s="1">
+        <v>-2.011525851630627</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-3.735473697833986</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
-        <v>0.4560650923999462</v>
-      </c>
-      <c r="B4">
-        <v>2.965131469512647</v>
+      <c r="A4" s="1">
+        <v>0.8528022432798865</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-2.876235097111638</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5">
-        <v>0.6437708258091843</v>
-      </c>
-      <c r="B5">
-        <v>4.1908422928854</v>
+      <c r="A5" s="1">
+        <v>1.196765323619466</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-4.0675979103375</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6">
-        <v>-1.139915732579205</v>
-      </c>
-      <c r="B6">
-        <v>-0.8370138120503995</v>
+      <c r="A6" s="1">
+        <v>-1.24293612056506</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.6746182617891435</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7">
-        <v>1.139847673863266</v>
-      </c>
-      <c r="B7">
-        <v>0.8371064922297693</v>
+      <c r="A7" s="1">
+        <v>1.242341834377565</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-0.6757120433291937</v>
       </c>
     </row>
   </sheetData>

</xml_diff>